<commit_message>
started on user part
</commit_message>
<xml_diff>
--- a/Data/KravSpecificationer.xlsx
+++ b/Data/KravSpecificationer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drage\source\repos\ApprenticeTest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3806835-96C8-4236-88F6-2FBE6E34DA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9480068A-18D3-4BE7-AB7A-2BEF7A784819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{040B1F35-3165-42A1-998F-8B6B05D0A6DD}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{040B1F35-3165-42A1-998F-8B6B05D0A6DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="148">
   <si>
     <t>Id</t>
   </si>
@@ -51,18 +51,6 @@
     <t>Entity factories, one for each aggregate root</t>
   </si>
   <si>
-    <t>Dish</t>
-  </si>
-  <si>
-    <t>Menu</t>
-  </si>
-  <si>
-    <t>Order</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
     <t>Brainstorm</t>
   </si>
   <si>
@@ -135,9 +123,6 @@
     <t>Cat-Repo-2</t>
   </si>
   <si>
-    <t>Entityframework Unit of Work with lock</t>
-  </si>
-  <si>
     <t>Cat-Repo-3</t>
   </si>
   <si>
@@ -313,6 +298,177 @@
   </si>
   <si>
     <t>All entity changes are logged</t>
+  </si>
+  <si>
+    <t>User-Repo-1</t>
+  </si>
+  <si>
+    <t>User-Repo-2</t>
+  </si>
+  <si>
+    <t>Entityframework Unit of Work</t>
+  </si>
+  <si>
+    <t>User-Repo-3</t>
+  </si>
+  <si>
+    <t>User EF repo</t>
+  </si>
+  <si>
+    <t>User-Service-1</t>
+  </si>
+  <si>
+    <t>Can create user</t>
+  </si>
+  <si>
+    <t>User-Service-2</t>
+  </si>
+  <si>
+    <t>User-Service-3</t>
+  </si>
+  <si>
+    <t>Can login</t>
+  </si>
+  <si>
+    <t>User-Service-4</t>
+  </si>
+  <si>
+    <t>Can place order</t>
+  </si>
+  <si>
+    <t>User-Service-5</t>
+  </si>
+  <si>
+    <t>Can see orders</t>
+  </si>
+  <si>
+    <t>Can add orders to menu</t>
+  </si>
+  <si>
+    <t>Can add orders to customer</t>
+  </si>
+  <si>
+    <t>Can produce Dish</t>
+  </si>
+  <si>
+    <t>Can produce Menu</t>
+  </si>
+  <si>
+    <t>Can produce Order</t>
+  </si>
+  <si>
+    <t>Can produce Customer</t>
+  </si>
+  <si>
+    <t>Can producer User</t>
+  </si>
+  <si>
+    <t>Security-1</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Can hash and salt password</t>
+  </si>
+  <si>
+    <t>User-Service-6</t>
+  </si>
+  <si>
+    <t>Can logout</t>
+  </si>
+  <si>
+    <t>Security-2</t>
+  </si>
+  <si>
+    <t>Security-3</t>
+  </si>
+  <si>
+    <t>REST-API middleware validats if user has logged in if needed</t>
+  </si>
+  <si>
+    <t>Can generate login JWT</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>Can get list of menues</t>
+  </si>
+  <si>
+    <t>User-Frontend</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Can create user if not logged in</t>
+  </si>
+  <si>
+    <t>Can login if not logged in</t>
+  </si>
+  <si>
+    <t>Can logout if logged in</t>
+  </si>
+  <si>
+    <t>Security-4</t>
+  </si>
+  <si>
+    <t>Validate all user input and sanitise as needed</t>
+  </si>
+  <si>
+    <t>Logged in user can see their orders</t>
+  </si>
+  <si>
+    <t>Logged in user can place orders</t>
+  </si>
+  <si>
+    <t>DDD</t>
+  </si>
+  <si>
+    <t>Cat-Rules-1</t>
+  </si>
+  <si>
+    <t>Menu cannot be modifed if future orders have been placed</t>
+  </si>
+  <si>
+    <t>User-Factory-1</t>
+  </si>
+  <si>
+    <t>Password is validated</t>
+  </si>
+  <si>
+    <t>Security-5</t>
+  </si>
+  <si>
+    <t>Can get salt from salted and hashed password</t>
+  </si>
+  <si>
+    <t>User-Endpoint-1</t>
+  </si>
+  <si>
+    <t>User-Endpoint-2</t>
+  </si>
+  <si>
+    <t>User-Endpoint-3</t>
+  </si>
+  <si>
+    <t>User-Endpoint-4</t>
+  </si>
+  <si>
+    <t>User-Endpoint-5</t>
+  </si>
+  <si>
+    <t>User-Endpoint-6</t>
+  </si>
+  <si>
+    <t>User-Frontend-1</t>
+  </si>
+  <si>
+    <t>User-Frontend-2</t>
+  </si>
+  <si>
+    <t>User-Frontend-3</t>
   </si>
 </sst>
 </file>
@@ -664,15 +820,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21638914-7399-4E98-8EB4-7F39ADF6EC4E}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -702,10 +858,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -714,279 +870,279 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -994,407 +1150,917 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
         <v>52</v>
       </c>
-      <c r="C24" t="s">
-        <v>57</v>
-      </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D33">
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="s">
         <v>75</v>
-      </c>
-      <c r="C35" t="s">
-        <v>80</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D41">
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D42">
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" t="s">
+        <v>106</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" t="s">
+        <v>100</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" t="s">
+        <v>102</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>143</v>
+      </c>
+      <c r="B62" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>144</v>
+      </c>
+      <c r="B63" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>145</v>
+      </c>
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" t="s">
+        <v>126</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>146</v>
+      </c>
+      <c r="B65" t="s">
+        <v>124</v>
+      </c>
+      <c r="C65" t="s">
+        <v>127</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>147</v>
+      </c>
+      <c r="B66" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" t="s">
+        <v>125</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>123</v>
+      </c>
+      <c r="B68" t="s">
+        <v>124</v>
+      </c>
+      <c r="C68" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>123</v>
+      </c>
+      <c r="B69" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" t="s">
+        <v>131</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" t="s">
+        <v>134</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>128</v>
+      </c>
+      <c r="B71" t="s">
+        <v>113</v>
+      </c>
+      <c r="C71" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>137</v>
+      </c>
+      <c r="B72" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" t="s">
+        <v>138</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
todo comments and schedule update
</commit_message>
<xml_diff>
--- a/Data/KravSpecificationer.xlsx
+++ b/Data/KravSpecificationer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drage\source\repos\ApprenticeTest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9480068A-18D3-4BE7-AB7A-2BEF7A784819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DCF3CA-F06D-4961-9D66-E1F2CD8E55EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{040B1F35-3165-42A1-998F-8B6B05D0A6DD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{040B1F35-3165-42A1-998F-8B6B05D0A6DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="151">
   <si>
     <t>Id</t>
   </si>
@@ -360,9 +360,6 @@
     <t>Can produce Customer</t>
   </si>
   <si>
-    <t>Can producer User</t>
-  </si>
-  <si>
     <t>Security-1</t>
   </si>
   <si>
@@ -469,6 +466,18 @@
   </si>
   <si>
     <t>User-Frontend-3</t>
+  </si>
+  <si>
+    <t>User-Factory-2</t>
+  </si>
+  <si>
+    <t>Can produce User</t>
+  </si>
+  <si>
+    <t>Can produce Token</t>
+  </si>
+  <si>
+    <t>JWT reading</t>
   </si>
 </sst>
 </file>
@@ -820,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21638914-7399-4E98-8EB4-7F39ADF6EC4E}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,13 +1734,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B53" t="s">
         <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -1742,13 +1751,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" t="s">
         <v>112</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>113</v>
-      </c>
-      <c r="C54" t="s">
-        <v>114</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -1759,13 +1768,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" t="s">
         <v>115</v>
-      </c>
-      <c r="B55" t="s">
-        <v>47</v>
-      </c>
-      <c r="C55" t="s">
-        <v>116</v>
       </c>
       <c r="D55">
         <v>3</v>
@@ -1776,13 +1785,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -1793,13 +1802,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" t="s">
         <v>118</v>
-      </c>
-      <c r="B57" t="s">
-        <v>113</v>
-      </c>
-      <c r="C57" t="s">
-        <v>119</v>
       </c>
       <c r="D57">
         <v>3</v>
@@ -1810,10 +1819,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C58" t="s">
         <v>100</v>
@@ -1827,13 +1836,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D59">
         <v>3</v>
@@ -1844,13 +1853,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B60" t="s">
+        <v>120</v>
+      </c>
+      <c r="C60" t="s">
         <v>121</v>
-      </c>
-      <c r="C60" t="s">
-        <v>122</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -1861,10 +1870,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C61" t="s">
         <v>102</v>
@@ -1878,10 +1887,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C62" t="s">
         <v>97</v>
@@ -1895,10 +1904,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C63" t="s">
         <v>104</v>
@@ -1912,13 +1921,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D64">
         <v>3</v>
@@ -1929,13 +1938,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D65">
         <v>3</v>
@@ -1946,13 +1955,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B66" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66" t="s">
         <v>124</v>
-      </c>
-      <c r="C66" t="s">
-        <v>125</v>
       </c>
       <c r="D66">
         <v>3</v>
@@ -1963,13 +1972,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" t="s">
+        <v>112</v>
+      </c>
+      <c r="C67" t="s">
         <v>128</v>
-      </c>
-      <c r="B67" t="s">
-        <v>113</v>
-      </c>
-      <c r="C67" t="s">
-        <v>129</v>
       </c>
       <c r="D67">
         <v>2</v>
@@ -1980,13 +1989,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>122</v>
+      </c>
+      <c r="B68" t="s">
         <v>123</v>
       </c>
-      <c r="B68" t="s">
-        <v>124</v>
-      </c>
       <c r="C68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D68">
         <v>3</v>
@@ -1997,13 +2006,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" t="s">
         <v>123</v>
       </c>
-      <c r="B69" t="s">
-        <v>124</v>
-      </c>
       <c r="C69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D69">
         <v>3</v>
@@ -2014,13 +2023,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>132</v>
+      </c>
+      <c r="B70" t="s">
+        <v>131</v>
+      </c>
+      <c r="C70" t="s">
         <v>133</v>
-      </c>
-      <c r="B70" t="s">
-        <v>132</v>
-      </c>
-      <c r="C70" t="s">
-        <v>134</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -2031,13 +2040,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B71" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -2048,19 +2057,36 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72" t="s">
         <v>137</v>
       </c>
-      <c r="B72" t="s">
-        <v>113</v>
-      </c>
-      <c r="C72" t="s">
-        <v>138</v>
-      </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" t="s">
+        <v>149</v>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rabbitmq communication for new api is ready, api is partly implemented, minor changes to some models
</commit_message>
<xml_diff>
--- a/Data/KravSpecificationer.xlsx
+++ b/Data/KravSpecificationer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drage\source\repos\ApprenticeTest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DCF3CA-F06D-4961-9D66-E1F2CD8E55EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1E4630-F180-462C-B150-246DDE0E9C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{040B1F35-3165-42A1-998F-8B6B05D0A6DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{040B1F35-3165-42A1-998F-8B6B05D0A6DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="201">
   <si>
     <t>Id</t>
   </si>
@@ -252,9 +252,6 @@
     <t>Cat-Com-2-a</t>
   </si>
   <si>
-    <t>Can ansswer RPC call for menues</t>
-  </si>
-  <si>
     <t>Cat-Service-12</t>
   </si>
   <si>
@@ -381,9 +378,6 @@
     <t>Security-3</t>
   </si>
   <si>
-    <t>REST-API middleware validats if user has logged in if needed</t>
-  </si>
-  <si>
     <t>Can generate login JWT</t>
   </si>
   <si>
@@ -478,6 +472,162 @@
   </si>
   <si>
     <t>JWT reading</t>
+  </si>
+  <si>
+    <t>Cat-Endpoint-1</t>
+  </si>
+  <si>
+    <t>Can get all menues</t>
+  </si>
+  <si>
+    <t>Cat-Endpoint-2</t>
+  </si>
+  <si>
+    <t>Can get all dishes</t>
+  </si>
+  <si>
+    <t>Cat-Endpoint-3</t>
+  </si>
+  <si>
+    <t>Cat-Endpoint-4</t>
+  </si>
+  <si>
+    <t>Can place menu</t>
+  </si>
+  <si>
+    <t>Can place dish</t>
+  </si>
+  <si>
+    <t>REST-API middleware validates if user has logged in if needed</t>
+  </si>
+  <si>
+    <t>User-Endpoint-7</t>
+  </si>
+  <si>
+    <t>Can update user</t>
+  </si>
+  <si>
+    <t>User-Frontend-4</t>
+  </si>
+  <si>
+    <t>User-Frontend-5</t>
+  </si>
+  <si>
+    <t>Can see all menues if logged in</t>
+  </si>
+  <si>
+    <t>Can update user if logged in</t>
+  </si>
+  <si>
+    <t>Cat-Endpoint-5</t>
+  </si>
+  <si>
+    <t>Cat-Factory-2</t>
+  </si>
+  <si>
+    <t>Can create employee</t>
+  </si>
+  <si>
+    <t>Requires being logged in to do</t>
+  </si>
+  <si>
+    <t>Cat-Service-16</t>
+  </si>
+  <si>
+    <t>Service for Employee</t>
+  </si>
+  <si>
+    <t>Cat-Repo-7</t>
+  </si>
+  <si>
+    <t>Employee EF repo</t>
+  </si>
+  <si>
+    <t>Can answer RPC call for menues</t>
+  </si>
+  <si>
+    <t>Cat-Com-2-b</t>
+  </si>
+  <si>
+    <t>Can answer RPC call for customer orders</t>
+  </si>
+  <si>
+    <t>Cat-Com-3-a</t>
+  </si>
+  <si>
+    <t>Cat-Com-3</t>
+  </si>
+  <si>
+    <t>Only got RPC calls</t>
+  </si>
+  <si>
+    <t>Can fetch dishes</t>
+  </si>
+  <si>
+    <t>Cat-Com-3-b</t>
+  </si>
+  <si>
+    <t>Can fetch menues</t>
+  </si>
+  <si>
+    <t>Cat-Com-3-c</t>
+  </si>
+  <si>
+    <t>Can create menues</t>
+  </si>
+  <si>
+    <t>Can create dishes</t>
+  </si>
+  <si>
+    <t>Cat-Com-3-d</t>
+  </si>
+  <si>
+    <t>Can fetch menues for display</t>
+  </si>
+  <si>
+    <t>Cat-Com-2-c</t>
+  </si>
+  <si>
+    <t>Cat-Com-2-d</t>
+  </si>
+  <si>
+    <t>Can create customer</t>
+  </si>
+  <si>
+    <t>Cat-Com-2-e</t>
+  </si>
+  <si>
+    <t>Cat-Com-2-f</t>
+  </si>
+  <si>
+    <t>Can update customer</t>
+  </si>
+  <si>
+    <t>Cat-Com-3-e</t>
+  </si>
+  <si>
+    <t>Can update user's location</t>
+  </si>
+  <si>
+    <t>Can update customer's location</t>
+  </si>
+  <si>
+    <t>Security-6</t>
+  </si>
+  <si>
+    <t>Employees have different roles</t>
+  </si>
+  <si>
+    <t>Security-6-a</t>
+  </si>
+  <si>
+    <t>Can only see orders</t>
+  </si>
+  <si>
+    <t>security-6-b</t>
+  </si>
+  <si>
+    <t>Can create and modify dishes and menues</t>
   </si>
 </sst>
 </file>
@@ -829,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21638914-7399-4E98-8EB4-7F39ADF6EC4E}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +1040,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -907,7 +1057,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -924,7 +1074,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -941,7 +1091,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1077,7 +1227,7 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1196,7 +1346,7 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -1434,7 +1584,7 @@
         <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>172</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -1445,13 +1595,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
         <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1462,13 +1612,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s">
         <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1479,13 +1629,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
         <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1496,13 +1646,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
         <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1513,13 +1663,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
         <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D40">
         <v>3</v>
@@ -1530,13 +1680,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
         <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D41">
         <v>3</v>
@@ -1547,13 +1697,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D42">
         <v>3</v>
@@ -1564,7 +1714,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B43" t="s">
         <v>20</v>
@@ -1581,13 +1731,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1598,13 +1748,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
         <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1615,13 +1765,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1632,7 +1782,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B47" t="s">
         <v>47</v>
@@ -1641,7 +1791,7 @@
         <v>50</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
@@ -1649,13 +1799,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -1666,13 +1816,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1683,13 +1833,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B50" t="s">
         <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -1700,13 +1850,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
         <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1717,13 +1867,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B52" t="s">
         <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -1734,13 +1884,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B53" t="s">
         <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -1751,13 +1901,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" t="s">
         <v>111</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>112</v>
-      </c>
-      <c r="C54" t="s">
-        <v>113</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -1768,13 +1918,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B55" t="s">
         <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D55">
         <v>3</v>
@@ -1785,13 +1935,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C56" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -1802,13 +1952,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C57" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="D57">
         <v>3</v>
@@ -1819,13 +1969,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -1836,13 +1986,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D59">
         <v>3</v>
@@ -1853,13 +2003,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B60" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C60" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -1870,13 +2020,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -1887,13 +2037,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C62" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -1904,13 +2054,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B63" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -1921,13 +2071,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B64" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" t="s">
         <v>123</v>
-      </c>
-      <c r="C64" t="s">
-        <v>125</v>
       </c>
       <c r="D64">
         <v>3</v>
@@ -1938,13 +2088,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C65" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D65">
         <v>3</v>
@@ -1955,13 +2105,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B66" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C66" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D66">
         <v>3</v>
@@ -1972,13 +2122,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D67">
         <v>2</v>
@@ -1989,13 +2139,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B68" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C68" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D68">
         <v>3</v>
@@ -2006,13 +2156,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B69" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C69" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D69">
         <v>3</v>
@@ -2023,13 +2173,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B70" t="s">
+        <v>129</v>
+      </c>
+      <c r="C70" t="s">
         <v>131</v>
-      </c>
-      <c r="C70" t="s">
-        <v>133</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -2040,13 +2190,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -2057,13 +2207,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C72" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -2074,19 +2224,481 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B73" t="s">
         <v>14</v>
       </c>
       <c r="C73" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D73">
         <v>3</v>
       </c>
       <c r="E73" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" t="s">
+        <v>118</v>
+      </c>
+      <c r="C74" t="s">
         <v>150</v>
+      </c>
+      <c r="D74">
+        <v>4</v>
+      </c>
+      <c r="E74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" t="s">
+        <v>118</v>
+      </c>
+      <c r="C75" t="s">
+        <v>152</v>
+      </c>
+      <c r="D75">
+        <v>4</v>
+      </c>
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76">
+        <v>4</v>
+      </c>
+      <c r="E76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
+        <v>118</v>
+      </c>
+      <c r="C77" t="s">
+        <v>155</v>
+      </c>
+      <c r="D77">
+        <v>4</v>
+      </c>
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>158</v>
+      </c>
+      <c r="B78" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" t="s">
+        <v>159</v>
+      </c>
+      <c r="D78">
+        <v>4</v>
+      </c>
+      <c r="E78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>160</v>
+      </c>
+      <c r="B79" t="s">
+        <v>121</v>
+      </c>
+      <c r="C79" t="s">
+        <v>163</v>
+      </c>
+      <c r="D79">
+        <v>4</v>
+      </c>
+      <c r="E79" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80" t="s">
+        <v>121</v>
+      </c>
+      <c r="C80" t="s">
+        <v>162</v>
+      </c>
+      <c r="D80">
+        <v>4</v>
+      </c>
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>164</v>
+      </c>
+      <c r="B81" t="s">
+        <v>118</v>
+      </c>
+      <c r="C81" t="s">
+        <v>99</v>
+      </c>
+      <c r="D81">
+        <v>99</v>
+      </c>
+      <c r="E81" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82" t="s">
+        <v>166</v>
+      </c>
+      <c r="D82">
+        <v>99</v>
+      </c>
+      <c r="E82" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>168</v>
+      </c>
+      <c r="B83" t="s">
+        <v>47</v>
+      </c>
+      <c r="C83" t="s">
+        <v>169</v>
+      </c>
+      <c r="D83">
+        <v>99</v>
+      </c>
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>170</v>
+      </c>
+      <c r="B84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" t="s">
+        <v>171</v>
+      </c>
+      <c r="D84">
+        <v>99</v>
+      </c>
+      <c r="E84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>173</v>
+      </c>
+      <c r="B85" t="s">
+        <v>70</v>
+      </c>
+      <c r="C85" t="s">
+        <v>174</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+      <c r="E85" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>176</v>
+      </c>
+      <c r="B86" t="s">
+        <v>70</v>
+      </c>
+      <c r="C86" t="s">
+        <v>177</v>
+      </c>
+      <c r="D86">
+        <v>4</v>
+      </c>
+      <c r="E86" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" t="s">
+        <v>70</v>
+      </c>
+      <c r="C87" t="s">
+        <v>178</v>
+      </c>
+      <c r="D87">
+        <v>4</v>
+      </c>
+      <c r="E87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" t="s">
+        <v>70</v>
+      </c>
+      <c r="C88" t="s">
+        <v>180</v>
+      </c>
+      <c r="D88">
+        <v>4</v>
+      </c>
+      <c r="E88" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>181</v>
+      </c>
+      <c r="B89" t="s">
+        <v>70</v>
+      </c>
+      <c r="C89" t="s">
+        <v>182</v>
+      </c>
+      <c r="D89">
+        <v>4</v>
+      </c>
+      <c r="E89" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>184</v>
+      </c>
+      <c r="B90" t="s">
+        <v>70</v>
+      </c>
+      <c r="C90" t="s">
+        <v>183</v>
+      </c>
+      <c r="D90">
+        <v>4</v>
+      </c>
+      <c r="E90" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>186</v>
+      </c>
+      <c r="B91" t="s">
+        <v>70</v>
+      </c>
+      <c r="C91" t="s">
+        <v>185</v>
+      </c>
+      <c r="D91">
+        <v>3</v>
+      </c>
+      <c r="E91" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>187</v>
+      </c>
+      <c r="B92" t="s">
+        <v>70</v>
+      </c>
+      <c r="C92" t="s">
+        <v>101</v>
+      </c>
+      <c r="D92">
+        <v>3</v>
+      </c>
+      <c r="E92" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>189</v>
+      </c>
+      <c r="B93" t="s">
+        <v>70</v>
+      </c>
+      <c r="C93" t="s">
+        <v>188</v>
+      </c>
+      <c r="D93">
+        <v>3</v>
+      </c>
+      <c r="E93" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>190</v>
+      </c>
+      <c r="B94" t="s">
+        <v>70</v>
+      </c>
+      <c r="C94" t="s">
+        <v>191</v>
+      </c>
+      <c r="D94">
+        <v>3</v>
+      </c>
+      <c r="E94" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>192</v>
+      </c>
+      <c r="B95" t="s">
+        <v>70</v>
+      </c>
+      <c r="C95" t="s">
+        <v>166</v>
+      </c>
+      <c r="D95">
+        <v>99</v>
+      </c>
+      <c r="E95" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96" t="s">
+        <v>47</v>
+      </c>
+      <c r="C96" t="s">
+        <v>194</v>
+      </c>
+      <c r="D96">
+        <v>3</v>
+      </c>
+      <c r="E96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>113</v>
+      </c>
+      <c r="B97" t="s">
+        <v>47</v>
+      </c>
+      <c r="C97" t="s">
+        <v>193</v>
+      </c>
+      <c r="D97">
+        <v>3</v>
+      </c>
+      <c r="E97" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>195</v>
+      </c>
+      <c r="B98" t="s">
+        <v>111</v>
+      </c>
+      <c r="C98" t="s">
+        <v>196</v>
+      </c>
+      <c r="D98">
+        <v>99</v>
+      </c>
+      <c r="E98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>197</v>
+      </c>
+      <c r="B99" t="s">
+        <v>111</v>
+      </c>
+      <c r="C99" t="s">
+        <v>198</v>
+      </c>
+      <c r="D99">
+        <v>99</v>
+      </c>
+      <c r="E99" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>199</v>
+      </c>
+      <c r="B100" t="s">
+        <v>111</v>
+      </c>
+      <c r="C100" t="s">
+        <v>200</v>
+      </c>
+      <c r="D100">
+        <v>99</v>
+      </c>
+      <c r="E100" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>